<commit_message>
add randomForest model use by final roundabout data in cj
</commit_message>
<xml_diff>
--- a/data/2017df.xlsx
+++ b/data/2017df.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10713"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\roundabout\roundabout_project\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yangdongjae/Desktop/2020/대외활동/2020년 공공 빅데이터 청년 인턴십/실무형 프로젝트/roundabout_project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2A79208-FD0A-624A-BDA9-07D5B4BEC5F6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9300"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -375,8 +376,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -699,20 +700,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="J64" sqref="J64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
-    <col min="1" max="1" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -762,7 +767,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>66</v>
       </c>
@@ -812,7 +817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -862,7 +867,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -912,7 +917,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>61</v>
       </c>
@@ -962,7 +967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>62</v>
       </c>
@@ -1012,7 +1017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>58</v>
       </c>
@@ -1062,7 +1067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -1112,7 +1117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -1162,7 +1167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>63</v>
       </c>
@@ -1212,7 +1217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -1262,7 +1267,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -1312,7 +1317,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>46</v>
       </c>
@@ -1362,7 +1367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>57</v>
       </c>
@@ -1412,7 +1417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>36</v>
       </c>
@@ -1462,7 +1467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -1512,7 +1517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:16">
       <c r="A17" t="s">
         <v>68</v>
       </c>
@@ -1562,7 +1567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:16">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1612,7 +1617,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:16">
       <c r="A19" t="s">
         <v>30</v>
       </c>
@@ -1662,7 +1667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:16">
       <c r="A20" t="s">
         <v>69</v>
       </c>
@@ -1712,7 +1717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:16">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -1762,7 +1767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:16">
       <c r="A22" t="s">
         <v>31</v>
       </c>
@@ -1812,7 +1817,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:16">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -1862,7 +1867,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:16">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -1912,7 +1917,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:16">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -1962,7 +1967,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:16">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -2012,7 +2017,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:16">
       <c r="A27" t="s">
         <v>60</v>
       </c>
@@ -2062,7 +2067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:16">
       <c r="A28" t="s">
         <v>40</v>
       </c>
@@ -2112,7 +2117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:16">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -2162,7 +2167,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:16">
       <c r="A30" t="s">
         <v>19</v>
       </c>
@@ -2212,7 +2217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:16">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -2262,7 +2267,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:16">
       <c r="A32" t="s">
         <v>1</v>
       </c>
@@ -2312,7 +2317,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:16">
       <c r="A33" t="s">
         <v>45</v>
       </c>
@@ -2362,7 +2367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:16">
       <c r="A34" t="s">
         <v>25</v>
       </c>
@@ -2412,7 +2417,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:16">
       <c r="A35" t="s">
         <v>51</v>
       </c>
@@ -2462,7 +2467,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:16">
       <c r="A36" t="s">
         <v>48</v>
       </c>
@@ -2512,7 +2517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:16">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -2562,7 +2567,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:16">
       <c r="A38" t="s">
         <v>49</v>
       </c>
@@ -2612,7 +2617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:16">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -2662,7 +2667,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:16">
       <c r="A40" t="s">
         <v>52</v>
       </c>
@@ -2712,7 +2717,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:16">
       <c r="A41" t="s">
         <v>11</v>
       </c>
@@ -2762,7 +2767,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:16">
       <c r="A42" t="s">
         <v>71</v>
       </c>
@@ -2812,7 +2817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:16">
       <c r="A43" t="s">
         <v>8</v>
       </c>
@@ -2862,7 +2867,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:16">
       <c r="A44" t="s">
         <v>47</v>
       </c>
@@ -2912,7 +2917,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:16">
       <c r="A45" t="s">
         <v>26</v>
       </c>
@@ -2962,7 +2967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:16">
       <c r="A46" t="s">
         <v>35</v>
       </c>
@@ -3012,7 +3017,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:16">
       <c r="A47" t="s">
         <v>22</v>
       </c>
@@ -3062,7 +3067,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:16">
       <c r="A48" t="s">
         <v>37</v>
       </c>
@@ -3112,7 +3117,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:16">
       <c r="A49" t="s">
         <v>38</v>
       </c>
@@ -3162,7 +3167,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:16">
       <c r="A50" t="s">
         <v>16</v>
       </c>
@@ -3212,7 +3217,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:16">
       <c r="A51" t="s">
         <v>43</v>
       </c>
@@ -3262,7 +3267,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:16">
       <c r="A52" t="s">
         <v>5</v>
       </c>
@@ -3312,7 +3317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:16">
       <c r="A53" t="s">
         <v>55</v>
       </c>
@@ -3362,7 +3367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:16">
       <c r="A54" t="s">
         <v>29</v>
       </c>
@@ -3412,7 +3417,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:16">
       <c r="A55" t="s">
         <v>4</v>
       </c>
@@ -3462,7 +3467,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:16">
       <c r="A56" t="s">
         <v>41</v>
       </c>
@@ -3512,7 +3517,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:16">
       <c r="A57" t="s">
         <v>42</v>
       </c>
@@ -3562,7 +3567,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:16">
       <c r="A58" t="s">
         <v>10</v>
       </c>
@@ -3612,7 +3617,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:16">
       <c r="A59" t="s">
         <v>44</v>
       </c>
@@ -3662,7 +3667,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:16">
       <c r="A60" t="s">
         <v>28</v>
       </c>
@@ -3712,7 +3717,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:16">
       <c r="A61" t="s">
         <v>13</v>
       </c>
@@ -3762,7 +3767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:16">
       <c r="A62" t="s">
         <v>2</v>
       </c>
@@ -3812,7 +3817,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:16">
       <c r="A63" t="s">
         <v>17</v>
       </c>
@@ -3862,7 +3867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:16">
       <c r="A64" t="s">
         <v>18</v>
       </c>
@@ -3912,7 +3917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:16">
       <c r="A65" t="s">
         <v>50</v>
       </c>
@@ -3962,7 +3967,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:16">
       <c r="A66" t="s">
         <v>3</v>
       </c>
@@ -4012,7 +4017,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:16">
       <c r="A67" t="s">
         <v>70</v>
       </c>
@@ -4062,7 +4067,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:16">
       <c r="A68" t="s">
         <v>39</v>
       </c>
@@ -4112,7 +4117,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:16">
       <c r="A69" t="s">
         <v>65</v>
       </c>
@@ -4162,7 +4167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:16">
       <c r="A70" t="s">
         <v>67</v>
       </c>
@@ -4212,7 +4217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:16">
       <c r="A71" t="s">
         <v>24</v>
       </c>
@@ -4263,7 +4268,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G71">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G71">
     <sortCondition ref="A1"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>